<commit_message>
76: Fixed one issue about LFL calculate. Named V0.31.
</commit_message>
<xml_diff>
--- a/Objects/PGS7-0-30_20250517-BurnFile/PGS7_FW_ChangeNote.xlsx
+++ b/Objects/PGS7-0-30_20250517-BurnFile/PGS7_FW_ChangeNote.xlsx
@@ -926,7 +926,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -934,6 +934,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1290,7 +1293,7 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="4"/>
@@ -1733,7 +1736,7 @@
       <c r="B31" t="s">
         <v>62</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="4" t="s">
         <v>65</v>
       </c>
       <c r="D31" t="s">

</xml_diff>